<commit_message>
added the latest set of results in an overall document
</commit_message>
<xml_diff>
--- a/Results/Scenario1-AllMembersLowExpertiseInAllSkills/ExpertiseBased/WithFigures/TeamStats.xlsx
+++ b/Results/Scenario1-AllMembersLowExpertiseInAllSkills/ExpertiseBased/WithFigures/TeamStats.xlsx
@@ -615,6 +615,21 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-NZ"/>
+              <a:t>Team Velocity - Expertise Based</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -811,11 +826,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="37924704"/>
-        <c:axId val="37918176"/>
+        <c:axId val="2083945744"/>
+        <c:axId val="2083952816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37924704"/>
+        <c:axId val="2083945744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -851,7 +866,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37918176"/>
+        <c:crossAx val="2083952816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -859,7 +874,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37918176"/>
+        <c:axId val="2083952816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,7 +885,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37924704"/>
+        <c:crossAx val="2083945744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -916,6 +931,26 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-NZ"/>
+              <a:t>Story Points - Expertise</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-NZ" baseline="0"/>
+              <a:t> Based</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-NZ"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -1105,11 +1140,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="37923072"/>
-        <c:axId val="37920896"/>
+        <c:axId val="2083946288"/>
+        <c:axId val="2083946832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37923072"/>
+        <c:axId val="2083946288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1145,7 +1180,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37920896"/>
+        <c:crossAx val="2083946832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1153,7 +1188,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37920896"/>
+        <c:axId val="2083946832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1164,7 +1199,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37923072"/>
+        <c:crossAx val="2083946288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1220,8 +1255,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-NZ"/>
-              <a:t>Active vs. Idle Time Periods</a:t>
+              <a:t>Active vs. Idle Time Periods - Expertise Based,</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-NZ" baseline="0"/>
+              <a:t> First Scenario</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-NZ"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1229,8 +1269,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.35917599594563093"/>
-          <c:y val="2.2884062133652293E-3"/>
+          <c:x val="0.17482994128298218"/>
+          <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1244,7 +1284,7 @@
           <c:yMode val="edge"/>
           <c:x val="6.4240763827198274E-2"/>
           <c:y val="9.0645211627121691E-2"/>
-          <c:w val="0.83664274937314043"/>
+          <c:w val="0.91433144383811393"/>
           <c:h val="0.80715600839971213"/>
         </c:manualLayout>
       </c:layout>
@@ -1518,11 +1558,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="37918720"/>
-        <c:axId val="37930144"/>
+        <c:axId val="2083947920"/>
+        <c:axId val="2083955536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="37918720"/>
+        <c:axId val="2083947920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1558,7 +1598,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37930144"/>
+        <c:crossAx val="2083955536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1566,7 +1606,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37930144"/>
+        <c:axId val="2083955536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80"/>
@@ -1604,21 +1644,21 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37918720"/>
+        <c:crossAx val="2083947920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.88087688586636015"/>
-          <c:y val="0.83776064856675481"/>
-          <c:w val="0.11750059928020019"/>
-          <c:h val="0.15599110152342985"/>
+          <c:x val="0.77948064594525768"/>
+          <c:y val="0.94946532379866777"/>
+          <c:w val="0.18895688334482125"/>
+          <c:h val="4.1381051347871262E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2002,7 +2042,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2423,7 +2463,10 @@
       <c r="A25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="5"/>
+      <c r="B25" s="5">
+        <f>AVERAGE(B2:B23)</f>
+        <v>1.4356585868003515</v>
+      </c>
       <c r="C25" s="5">
         <f>AVERAGE(C2:C23)</f>
         <v>99.545454545454547</v>

</xml_diff>

<commit_message>
alterations to the results figures
</commit_message>
<xml_diff>
--- a/Results/Scenario1-AllMembersLowExpertiseInAllSkills/ExpertiseBased/WithFigures/TeamStats.xlsx
+++ b/Results/Scenario1-AllMembersLowExpertiseInAllSkills/ExpertiseBased/WithFigures/TeamStats.xlsx
@@ -826,11 +826,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2083945744"/>
-        <c:axId val="2083952816"/>
+        <c:axId val="-71581392"/>
+        <c:axId val="-71569968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2083945744"/>
+        <c:axId val="-71581392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -866,7 +866,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083952816"/>
+        <c:crossAx val="-71569968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -874,7 +874,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2083952816"/>
+        <c:axId val="-71569968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -885,7 +885,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083945744"/>
+        <c:crossAx val="-71581392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1140,11 +1140,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2083946288"/>
-        <c:axId val="2083946832"/>
+        <c:axId val="-71579760"/>
+        <c:axId val="-71577584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2083946288"/>
+        <c:axId val="-71579760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1180,7 +1180,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083946832"/>
+        <c:crossAx val="-71577584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1188,7 +1188,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2083946832"/>
+        <c:axId val="-71577584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1199,7 +1199,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083946288"/>
+        <c:crossAx val="-71579760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1558,11 +1558,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2083947920"/>
-        <c:axId val="2083955536"/>
+        <c:axId val="-71579216"/>
+        <c:axId val="-71580304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2083947920"/>
+        <c:axId val="-71579216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1598,7 +1598,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083955536"/>
+        <c:crossAx val="-71580304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1606,7 +1606,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2083955536"/>
+        <c:axId val="-71580304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80"/>
@@ -1644,7 +1644,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083947920"/>
+        <c:crossAx val="-71579216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1659,6 +1659,508 @@
           <c:y val="0.94946532379866777"/>
           <c:w val="0.18895688334482125"/>
           <c:h val="4.1381051347871262E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-NZ"/>
+              <a:t>Team Velocity vs Story</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-NZ" baseline="0"/>
+              <a:t> Points</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-NZ"/>
+              <a:t> - Expertise Based</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12711967112419434"/>
+          <c:y val="9.5808371187279459E-3"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.5833274006327852E-2"/>
+          <c:y val="0.13412493009257956"/>
+          <c:w val="0.86648807858317178"/>
+          <c:h val="0.73392707700478388"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Story Points</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>TeamStats!$C$2:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>238</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>197</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-42584288"/>
+        <c:axId val="-42593536"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Team Velocity</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>TeamStats!$A$2:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TeamStats!$B$2:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.73751684452052302</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.64902646030953504</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21220291591771501</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39973351099267102</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.39946737683089201</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.42138338604960801</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.66570509264395805</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.57475094125878701</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.73448171956608999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4853089442603999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.49774025155029</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.8214055448098001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.06898519843232</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.0098202396804199</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.6810475580572299</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.71595410463051</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.2445279391847599</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.0802588105726798</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.0481685900652198</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.0058601643540301</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.4887144589677899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-42588640"/>
+        <c:axId val="-1945379568"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-42584288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-NZ" sz="2000" b="0"/>
+                  <a:t>Sprints</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.42439405194419311"/>
+              <c:y val="0.9097339293401947"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-42593536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-42593536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-42584288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1945379568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-42588640"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="-42588640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1945379568"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.75183469454318486"/>
+          <c:y val="0.74094548025894913"/>
+          <c:w val="0.18400439075028518"/>
+          <c:h val="0.11549963185444773"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1768,6 +2270,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>33618</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>43423</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2041,8 +2575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S41" sqref="S41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q51" sqref="Q51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
resolved some minor problems with the results
</commit_message>
<xml_diff>
--- a/Results/Scenario1-AllMembersLowExpertiseInAllSkills/ExpertiseBased/WithFigures/TeamStats.xlsx
+++ b/Results/Scenario1-AllMembersLowExpertiseInAllSkills/ExpertiseBased/WithFigures/TeamStats.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\CourseWork\GitHubRepositories\AgileSoftwareModel\AgileSoftwareModel\Results\Scenario1-AllMembersLowExpertiseInAllSkills\ExpertiseBased\WithFigures\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
@@ -603,7 +598,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-NZ"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -825,12 +820,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-71581392"/>
-        <c:axId val="-71569968"/>
+        <c:axId val="108799488"/>
+        <c:axId val="108801408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-71581392"/>
+        <c:axId val="108799488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -866,7 +862,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-71569968"/>
+        <c:crossAx val="108801408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -874,7 +870,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-71569968"/>
+        <c:axId val="108801408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -885,7 +881,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-71581392"/>
+        <c:crossAx val="108799488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -919,7 +915,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-NZ"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1139,12 +1135,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-71579760"/>
-        <c:axId val="-71577584"/>
+        <c:axId val="108838272"/>
+        <c:axId val="108840448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-71579760"/>
+        <c:axId val="108838272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1180,7 +1177,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-71577584"/>
+        <c:crossAx val="108840448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1188,7 +1185,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-71577584"/>
+        <c:axId val="108840448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1199,7 +1196,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-71579760"/>
+        <c:crossAx val="108838272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1233,7 +1230,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-NZ"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1558,11 +1555,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-71579216"/>
-        <c:axId val="-71580304"/>
+        <c:axId val="109214336"/>
+        <c:axId val="109224704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-71579216"/>
+        <c:axId val="109214336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1598,7 +1595,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-71580304"/>
+        <c:crossAx val="109224704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1606,7 +1603,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-71580304"/>
+        <c:axId val="109224704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80"/>
@@ -1644,7 +1641,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-71579216"/>
+        <c:crossAx val="109214336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1678,7 +1675,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-NZ"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1740,6 +1737,187 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Team Velocity</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>TeamStats!$A$2:$A$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TeamStats!$B$2:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0.73751684452052302</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.64902646030953504</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21220291591771501</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39973351099267102</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.39946737683089201</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.42138338604960801</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.66570509264395805</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.57475094125878701</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.73448171956608999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4853089442603999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.49774025155029</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.8214055448098001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.06898519843232</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.0098202396804199</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.6810475580572299</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.71595410463051</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.2445279391847599</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.0802588105726798</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.0481685900652198</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.0058601643540301</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.4887144589677899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="109513728"/>
+        <c:axId val="109520000"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
@@ -1839,192 +2017,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-42584288"/>
-        <c:axId val="-42593536"/>
-      </c:lineChart>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Team Velocity</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>TeamStats!$A$2:$A$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>TeamStats!$B$2:$B$22</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>0.73751684452052302</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.64902646030953504</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.21220291591771501</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.39973351099267102</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.39946737683089201</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.42138338604960801</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.66570509264395805</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.57475094125878701</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.73448171956608999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.4853089442603999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.49774025155029</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.8214055448098001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2.06898519843232</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.0098202396804199</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.6810475580572299</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.71595410463051</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.2445279391847599</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.0802588105726798</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.0481685900652198</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.0058601643540301</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.4887144589677899</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="-42588640"/>
-        <c:axId val="-1945379568"/>
+        <c:axId val="45656704"/>
+        <c:axId val="45654400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-42584288"/>
+        <c:axId val="109513728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2060,7 +2057,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-42593536"/>
+        <c:crossAx val="109520000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2068,14 +2065,14 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-42593536"/>
+        <c:axId val="109520000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2093,28 +2090,21 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-42584288"/>
+        <c:crossAx val="109513728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1945379568"/>
+        <c:axId val="45654400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -2129,22 +2119,21 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-42588640"/>
+        <c:crossAx val="45656704"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-42588640"/>
+        <c:axId val="45656704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1945379568"/>
+        <c:crossAx val="45654400"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2565,7 +2554,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2575,8 +2564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q51" sqref="Q51"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U52" sqref="U52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>